<commit_message>
Configuracion de importacion para asignar estudiantes
</commit_message>
<xml_diff>
--- a/public/asignacionStudent.xlsx
+++ b/public/asignacionStudent.xlsx
@@ -5,42 +5,68 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\narut\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13d2ad5f67de6611/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808AEE78-5680-4879-B00A-1DA2FAA97730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{32C85B41-6F1F-4D77-B66A-768EEE2B442E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B9EFB58-3FD1-4693-B4EA-8BDBEDF0B0DC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C1531AC2-F34C-450B-B138-45E9EAA5FB07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C6824096-AEFD-469D-B539-553F09206511}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>testeusertest4</t>
+  </si>
+  <si>
+    <t>testeusertest5</t>
+  </si>
+  <si>
+    <t>testeusertest6</t>
+  </si>
+  <si>
+    <t>testeusertest7</t>
+  </si>
+  <si>
+    <t>testeusertest8</t>
+  </si>
+  <si>
+    <t>testeusertest9</t>
+  </si>
+  <si>
+    <t>testeusertest10</t>
+  </si>
   <si>
     <t>classroom</t>
-  </si>
-  <si>
-    <t>user_name</t>
-  </si>
-  <si>
-    <t>SaraSofia2006</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,19 +80,21 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,17 +106,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,33 +430,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99F327A-920D-4098-AFF7-B76F1AAC16A2}">
-  <dimension ref="A1:B115"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FB0E3E-2C2F-402E-BA09-77ABE181763B}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="1"/>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>